<commit_message>
new lecture and small edits
</commit_message>
<xml_diff>
--- a/GradeCalcCS135.xlsx
+++ b/GradeCalcCS135.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sudo/CodeProjects/Tufts/CS0135/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE0BD9F2-061E-A149-8A5A-781A95E6F34D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C479D30-05D6-AF46-949F-78EF2B691B05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1020" yWindow="880" windowWidth="34980" windowHeight="22500" xr2:uid="{CEDA9B79-AA12-3148-A57D-A1F1ACAD8C6A}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>HW1</t>
   </si>
@@ -136,6 +135,9 @@
   </si>
   <si>
     <t>skipped</t>
+  </si>
+  <si>
+    <t>???</t>
   </si>
 </sst>
 </file>
@@ -571,7 +573,7 @@
   <dimension ref="A2:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="191" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -674,7 +676,7 @@
         <v>44997</v>
       </c>
       <c r="B5" s="8">
-        <v>45012</v>
+        <v>45014</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -756,11 +758,11 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="12">
-        <v>44999</v>
-      </c>
-      <c r="B12" s="8">
-        <v>45014</v>
+      <c r="A12" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
cleanup but svm element mismatch still
</commit_message>
<xml_diff>
--- a/GradeCalcCS135.xlsx
+++ b/GradeCalcCS135.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sudo/CodeProjects/Tufts/CS0135/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA7408F-E0B2-F849-A229-DDE2E944C25E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF76D192-DB54-AE4C-92C8-1B7674EBB1A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="880" windowWidth="35000" windowHeight="22500" xr2:uid="{CEDA9B79-AA12-3148-A57D-A1F1ACAD8C6A}"/>
   </bookViews>
@@ -599,7 +599,7 @@
   <dimension ref="A2:P27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="191" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -736,7 +736,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="12">
-        <v>45015</v>
+        <v>45021</v>
       </c>
       <c r="B6" s="8">
         <v>45029</v>

</xml_diff>

<commit_message>
final of mine before group merge
</commit_message>
<xml_diff>
--- a/GradeCalcCS135.xlsx
+++ b/GradeCalcCS135.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sudo/CodeProjects/Tufts/CS0135/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3D562AB-BF8C-AA42-9592-7952EE0298E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48BE3282-31D7-C141-B172-CAA2C6029CBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="880" windowWidth="35000" windowHeight="22500" xr2:uid="{CEDA9B79-AA12-3148-A57D-A1F1ACAD8C6A}"/>
   </bookViews>
@@ -199,7 +199,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -219,12 +219,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -273,10 +267,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="4"/>
-    <xf numFmtId="16" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="3"/>
     <xf numFmtId="10" fontId="3" fillId="3" borderId="0" xfId="3" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
@@ -599,7 +591,7 @@
   <dimension ref="A2:P27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="191" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -741,7 +733,7 @@
       <c r="B6" s="12">
         <v>45033</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="15" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="4"/>
@@ -813,11 +805,11 @@
       <c r="G10">
         <v>0.25</v>
       </c>
-      <c r="H10" s="15">
+      <c r="H10" s="14">
         <f>F10*G10</f>
         <v>0.24374999999999999</v>
       </c>
-      <c r="I10" s="15">
+      <c r="I10" s="14">
         <f>H10</f>
         <v>0.24374999999999999</v>
       </c>
@@ -827,16 +819,16 @@
       <c r="L10" s="10"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A12" s="12">
+      <c r="A12" s="11">
         <v>45015</v>
       </c>
-      <c r="B12" s="14">
-        <v>45027</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="B12" s="11">
+        <v>45029</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="4" t="s">
         <v>26</v>
       </c>
       <c r="G12">

</xml_diff>

<commit_message>
added functions for bonus
</commit_message>
<xml_diff>
--- a/GradeCalcCS135.xlsx
+++ b/GradeCalcCS135.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sudo/CodeProjects/Tufts/CS0135/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D11BEEEF-FFEB-814A-AC15-7B0175896628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1070A6C0-8068-3C46-A512-0738959A4F84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="760" windowWidth="29240" windowHeight="18880" xr2:uid="{CEDA9B79-AA12-3148-A57D-A1F1ACAD8C6A}"/>
+    <workbookView xWindow="1020" yWindow="880" windowWidth="30100" windowHeight="21980" xr2:uid="{CEDA9B79-AA12-3148-A57D-A1F1ACAD8C6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
   <si>
     <t>HW1</t>
   </si>
@@ -151,6 +151,9 @@
   </si>
   <si>
     <t>35/34 coding</t>
+  </si>
+  <si>
+    <t>40/40 code?</t>
   </si>
 </sst>
 </file>
@@ -160,7 +163,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -189,15 +192,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -214,11 +210,6 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -229,14 +220,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -261,12 +251,10 @@
     <xf numFmtId="16" fontId="2" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="3" fillId="3" borderId="0" xfId="3" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="5">
-    <cellStyle name="Bad" xfId="4" builtinId="27"/>
+  <cellStyles count="4">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -584,8 +572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5731E5A4-4C2E-EC43-B747-67AC75025145}">
   <dimension ref="A2:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="166" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="166" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -820,11 +808,11 @@
       <c r="G10">
         <v>0.25</v>
       </c>
-      <c r="H10" s="13">
+      <c r="H10" s="12">
         <f>F10*G10</f>
         <v>0.24374999999999999</v>
       </c>
-      <c r="I10" s="13">
+      <c r="I10" s="12">
         <f>H10</f>
         <v>0.24374999999999999</v>
       </c>
@@ -843,14 +831,28 @@
       <c r="C12" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>23</v>
+      <c r="D12" s="4">
+        <v>55.5</v>
+      </c>
+      <c r="E12" s="4">
+        <v>60</v>
+      </c>
+      <c r="F12" s="5">
+        <f>D12/E12</f>
+        <v>0.92500000000000004</v>
       </c>
       <c r="G12">
         <v>0.15</v>
       </c>
+      <c r="H12">
+        <f>F12*G12</f>
+        <v>0.13875000000000001</v>
+      </c>
       <c r="L12" t="s">
         <v>21</v>
+      </c>
+      <c r="M12" s="10" t="s">
+        <v>38</v>
       </c>
       <c r="N12" t="s">
         <v>25</v>
@@ -872,7 +874,17 @@
       <c r="C13" t="s">
         <v>5</v>
       </c>
+      <c r="D13" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="G13">
+        <v>0.15</v>
+      </c>
+      <c r="I13">
+        <f>H12+H13</f>
+        <v>0.13875000000000001</v>
+      </c>
+      <c r="J13" s="3">
         <v>0.15</v>
       </c>
       <c r="L13" t="s">
@@ -886,7 +898,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
-      <c r="K14" s="12"/>
+      <c r="K14" s="1"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="G15" s="3">
@@ -908,6 +920,12 @@
       <c r="C17" t="s">
         <v>7</v>
       </c>
+      <c r="D17">
+        <v>100</v>
+      </c>
+      <c r="E17">
+        <v>100</v>
+      </c>
       <c r="G17" s="3">
         <v>0.1</v>
       </c>
@@ -937,13 +955,13 @@
       <c r="H20" s="1">
         <v>1</v>
       </c>
-      <c r="I20" s="14">
+      <c r="I20" s="13">
         <f>SUM(I2:I19)</f>
-        <v>0.61138767165115204</v>
-      </c>
-      <c r="J20" s="14">
+        <v>0.75013767165115208</v>
+      </c>
+      <c r="J20" s="13">
         <f>SUM(J3:J19)</f>
-        <v>0.61249999999999993</v>
+        <v>0.76249999999999996</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
autograder 50/80 on proj2
</commit_message>
<xml_diff>
--- a/GradeCalcCS135.xlsx
+++ b/GradeCalcCS135.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sudo/CodeProjects/Tufts/CS0135/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1070A6C0-8068-3C46-A512-0738959A4F84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FFEF697-262F-AA40-9362-6D571F97B2E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1020" yWindow="880" windowWidth="30100" windowHeight="21980" xr2:uid="{CEDA9B79-AA12-3148-A57D-A1F1ACAD8C6A}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>HW1</t>
   </si>
@@ -573,7 +573,7 @@
   <dimension ref="A2:P27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="166" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -732,14 +732,21 @@
       <c r="C6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="4"/>
+      <c r="D6" s="4">
+        <v>41</v>
+      </c>
+      <c r="E6" s="4">
+        <v>41</v>
+      </c>
+      <c r="F6" s="5">
+        <f>D6/E6</f>
+        <v>1</v>
+      </c>
       <c r="G6">
+        <v>8.7499999999999994E-2</v>
+      </c>
+      <c r="H6">
+        <f>G6*F6</f>
         <v>8.7499999999999994E-2</v>
       </c>
       <c r="L6" t="s">
@@ -764,11 +771,11 @@
       <c r="F7" s="4"/>
       <c r="I7" s="6">
         <f>SUM(H3:H7)</f>
-        <v>0.26763767165115204</v>
+        <v>0.35513767165115206</v>
       </c>
       <c r="J7" s="6">
-        <f>SUM(G3:G5)</f>
-        <v>0.26249999999999996</v>
+        <f>SUM(G3:G6)</f>
+        <v>0.35</v>
       </c>
       <c r="K7" s="6"/>
       <c r="L7" t="s">
@@ -957,11 +964,11 @@
       </c>
       <c r="I20" s="13">
         <f>SUM(I2:I19)</f>
-        <v>0.75013767165115208</v>
+        <v>0.8376376716511521</v>
       </c>
       <c r="J20" s="13">
         <f>SUM(J3:J19)</f>
-        <v>0.76249999999999996</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
autograder 70/80 on proj2
</commit_message>
<xml_diff>
--- a/GradeCalcCS135.xlsx
+++ b/GradeCalcCS135.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sudo/CodeProjects/Tufts/CS0135/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FFEF697-262F-AA40-9362-6D571F97B2E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E24DB87B-0BAB-1945-AF64-894BEEAB48FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1020" yWindow="880" windowWidth="30100" windowHeight="21980" xr2:uid="{CEDA9B79-AA12-3148-A57D-A1F1ACAD8C6A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="41">
   <si>
     <t>HW1</t>
   </si>
@@ -154,6 +155,12 @@
   </si>
   <si>
     <t>40/40 code?</t>
+  </si>
+  <si>
+    <t>31/31 code</t>
+  </si>
+  <si>
+    <t>10/10 written</t>
   </si>
 </sst>
 </file>
@@ -569,10 +576,451 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEC16B75-CD82-C841-A21B-5B79A820F805}">
+  <dimension ref="A2:P27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="166" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.6640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="7"/>
+    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15" customWidth="1"/>
+    <col min="13" max="13" width="14.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3" s="11">
+        <v>44957</v>
+      </c>
+      <c r="B3" s="11">
+        <v>44971</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>83.75</v>
+      </c>
+      <c r="E3" s="4">
+        <v>76.5</v>
+      </c>
+      <c r="F3" s="5">
+        <f>D3/E3</f>
+        <v>1.0947712418300655</v>
+      </c>
+      <c r="G3">
+        <v>8.7499999999999994E-2</v>
+      </c>
+      <c r="H3" s="6">
+        <f>F3*G3</f>
+        <v>9.5792483660130726E-2</v>
+      </c>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="L3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" s="11">
+        <v>44971</v>
+      </c>
+      <c r="B4" s="11">
+        <v>44985</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4">
+        <v>79</v>
+      </c>
+      <c r="E4" s="4">
+        <v>81</v>
+      </c>
+      <c r="F4" s="5">
+        <f>D4/E4</f>
+        <v>0.97530864197530864</v>
+      </c>
+      <c r="G4">
+        <v>8.7499999999999994E-2</v>
+      </c>
+      <c r="H4" s="6">
+        <f>F4*G4</f>
+        <v>8.5339506172839502E-2</v>
+      </c>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="L4" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" s="11">
+        <v>44997</v>
+      </c>
+      <c r="B5" s="11">
+        <v>45015</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="4">
+        <v>87</v>
+      </c>
+      <c r="E5" s="4">
+        <v>88</v>
+      </c>
+      <c r="F5" s="5">
+        <f>D5/E5</f>
+        <v>0.98863636363636365</v>
+      </c>
+      <c r="G5">
+        <v>8.7499999999999994E-2</v>
+      </c>
+      <c r="H5" s="6">
+        <f>F5*G5</f>
+        <v>8.6505681818181815E-2</v>
+      </c>
+      <c r="L5" t="s">
+        <v>37</v>
+      </c>
+      <c r="M5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" s="11">
+        <v>45022</v>
+      </c>
+      <c r="B6" s="11">
+        <v>45033</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="4">
+        <v>41</v>
+      </c>
+      <c r="E6" s="4">
+        <v>41</v>
+      </c>
+      <c r="F6" s="5">
+        <f>D6/E6</f>
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>8.7499999999999994E-2</v>
+      </c>
+      <c r="H6">
+        <f>G6*F6</f>
+        <v>8.7499999999999994E-2</v>
+      </c>
+      <c r="L6" t="s">
+        <v>39</v>
+      </c>
+      <c r="M6" t="s">
+        <v>40</v>
+      </c>
+      <c r="N6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" s="8">
+        <v>45041</v>
+      </c>
+      <c r="B7" s="8">
+        <v>45051</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="I7" s="6">
+        <f>SUM(H3:H7)</f>
+        <v>0.35513767165115206</v>
+      </c>
+      <c r="J7" s="6">
+        <f>SUM(G3:G6)</f>
+        <v>0.35</v>
+      </c>
+      <c r="K7" s="6"/>
+      <c r="L7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="G8">
+        <v>0.35</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0.35</v>
+      </c>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" s="11">
+        <v>44994</v>
+      </c>
+      <c r="B10" s="11">
+        <v>44995</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="4">
+        <v>97.5</v>
+      </c>
+      <c r="E10" s="4">
+        <v>100</v>
+      </c>
+      <c r="F10" s="5">
+        <f>D10/E10</f>
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="G10">
+        <v>0.25</v>
+      </c>
+      <c r="H10" s="12">
+        <f>F10*G10</f>
+        <v>0.24374999999999999</v>
+      </c>
+      <c r="I10" s="12">
+        <f>H10</f>
+        <v>0.24374999999999999</v>
+      </c>
+      <c r="J10">
+        <v>0.25</v>
+      </c>
+      <c r="L10" s="10"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" s="11">
+        <v>45015</v>
+      </c>
+      <c r="B12" s="11">
+        <v>45029</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="4">
+        <v>55.5</v>
+      </c>
+      <c r="E12" s="4">
+        <v>60</v>
+      </c>
+      <c r="F12" s="5">
+        <f>D12/E12</f>
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="G12">
+        <v>0.15</v>
+      </c>
+      <c r="H12">
+        <f>F12*G12</f>
+        <v>0.13875000000000001</v>
+      </c>
+      <c r="L12" t="s">
+        <v>21</v>
+      </c>
+      <c r="M12" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="N12" t="s">
+        <v>25</v>
+      </c>
+      <c r="O12" t="s">
+        <v>26</v>
+      </c>
+      <c r="P12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" s="8">
+        <v>45039</v>
+      </c>
+      <c r="B13" s="8">
+        <v>45051</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13">
+        <v>0.15</v>
+      </c>
+      <c r="I13">
+        <f>H12+H13</f>
+        <v>0.13875000000000001</v>
+      </c>
+      <c r="J13" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="L13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="G15" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17">
+        <v>100</v>
+      </c>
+      <c r="E17">
+        <v>100</v>
+      </c>
+      <c r="G17" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="I17" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="J17" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="L17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G20" s="3">
+        <v>1</v>
+      </c>
+      <c r="H20" s="1">
+        <v>1</v>
+      </c>
+      <c r="I20" s="13">
+        <f>SUM(I2:I19)</f>
+        <v>0.8376376716511521</v>
+      </c>
+      <c r="J20" s="13">
+        <f>SUM(J3:J19)</f>
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="10"/>
+      <c r="L23" t="s">
+        <v>17</v>
+      </c>
+      <c r="N23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E24" s="10"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K26" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K27" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5731E5A4-4C2E-EC43-B747-67AC75025145}">
   <dimension ref="A2:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="166" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="166" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>

</xml_diff>